<commit_message>
EPBDS-11247 use Integer.valueOf instead of deprecated constructor
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11247_DecisionTableRetActionValidation.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11247_DecisionTableRetActionValidation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\openl-from-git\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE28B06-802E-44A0-B808-1AD10BE7708F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A835AB09-7430-4B77-B422-7434D5536A72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{69DD8098-E143-4884-9C95-043F2CD09D2E}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="27">
   <si>
     <t>C1</t>
   </si>
@@ -89,18 +89,12 @@
     <t>Integer[]</t>
   </si>
   <si>
-    <t>= new Integer (20)</t>
-  </si>
-  <si>
     <t>= 30.2</t>
   </si>
   <si>
     <t>= null</t>
   </si>
   <si>
-    <t>= new Integer (200)</t>
-  </si>
-  <si>
     <t>= 300</t>
   </si>
   <si>
@@ -108,6 +102,15 @@
   </si>
   <si>
     <t>Rules String[] ruleOutputCast5(Integer a)</t>
+  </si>
+  <si>
+    <t>= Integer.valueOf(20)</t>
+  </si>
+  <si>
+    <t>=  Integer.valueOf(20)</t>
+  </si>
+  <si>
+    <t>=  Integer.valueOf(200)</t>
   </si>
 </sst>
 </file>
@@ -146,14 +149,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -169,9 +172,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -209,7 +212,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -315,7 +318,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -467,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6D4758-B2C4-42D9-A25E-F7FB14D6933A}">
   <dimension ref="B2:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,10 +482,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -538,10 +541,10 @@
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -597,20 +600,20 @@
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1"/>
+      <c r="C28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -670,20 +673,20 @@
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1"/>
+      <c r="C39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
@@ -743,10 +746,10 @@
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="1"/>
+      <c r="C50" s="3"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
@@ -802,10 +805,10 @@
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C61" s="1"/>
+      <c r="C61" s="3"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
@@ -861,189 +864,197 @@
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="1">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="D77" s="1">
+        <v>100.33</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="1">
+        <v>2</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D78" s="1"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="1">
+        <v>3</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="1">
+        <v>4</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="1">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="1">
+        <v>6</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="1">
+        <v>7</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D90" s="3"/>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="1">
+        <v>1</v>
+      </c>
+      <c r="C92" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="D92" s="1">
+        <v>100.33</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="1">
+        <v>2</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="1"/>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D75" s="1"/>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D76" s="1"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="2">
-        <v>1</v>
-      </c>
-      <c r="C77" s="2">
-        <v>10.1</v>
-      </c>
-      <c r="D77" s="2">
-        <v>100.33</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="2">
-        <v>2</v>
-      </c>
-      <c r="C78" s="3" t="s">
+      <c r="D93" s="1"/>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="1">
+        <v>3</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="2">
-        <v>3</v>
-      </c>
-      <c r="C79" s="3" t="s">
+      <c r="D94" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="2">
-        <v>4</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="2">
-        <v>5</v>
-      </c>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="2">
-        <v>6</v>
-      </c>
-      <c r="C82" s="2"/>
-      <c r="D82" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="2">
-        <v>7</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D88" s="1"/>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D90" s="1"/>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D91" s="1"/>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="2">
-        <v>1</v>
-      </c>
-      <c r="C92" s="2">
-        <v>10.1</v>
-      </c>
-      <c r="D92" s="2">
-        <v>100.33</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="2">
-        <v>2</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D93" s="2"/>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="2">
-        <v>3</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B27:D27"/>
     <mergeCell ref="C88:D88"/>
     <mergeCell ref="C90:D90"/>
     <mergeCell ref="C91:D91"/>
@@ -1052,14 +1063,6 @@
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="C76:D76"/>
     <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B27:D27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>